<commit_message>
closing dates were wrong for algo
</commit_message>
<xml_diff>
--- a/Daily Backup hourlys/30 min csh/ADANI.xlsx
+++ b/Daily Backup hourlys/30 min csh/ADANI.xlsx
@@ -586,19 +586,19 @@
       <c r="D7" s="1" t="n"/>
       <c r="E7" s="1" t="n"/>
       <c r="F7" s="2" t="n">
-        <v>2188.7</v>
+        <v>2801.7</v>
       </c>
       <c r="G7" s="1" t="n">
-        <v>2194</v>
+        <v>2821.95</v>
       </c>
       <c r="H7" s="1" t="n">
-        <v>2153.5</v>
+        <v>2767.1</v>
       </c>
       <c r="I7" s="1" t="n">
-        <v>2172.65</v>
+        <v>2799.75</v>
       </c>
       <c r="J7" s="1" t="n">
-        <v>2196.65</v>
+        <v>2783.85</v>
       </c>
       <c r="K7" s="1" t="n"/>
       <c r="L7" s="1" t="n"/>
@@ -649,13 +649,13 @@
         <v>0.3958333333333333</v>
       </c>
       <c r="G9" s="1" t="n">
-        <v>2225</v>
+        <v>2817.8</v>
       </c>
       <c r="H9" s="1" t="n">
-        <v>2181.8</v>
+        <v>2725</v>
       </c>
       <c r="I9" s="1" t="n">
-        <v>2184.8</v>
+        <v>2782.9</v>
       </c>
       <c r="J9" s="1" t="n"/>
       <c r="K9" s="1" t="n"/>
@@ -674,13 +674,13 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="G10" s="1" t="n">
-        <v>2186</v>
+        <v>2810</v>
       </c>
       <c r="H10" s="1" t="n">
-        <v>2176.5</v>
+        <v>2772</v>
       </c>
       <c r="I10" s="1" t="n">
-        <v>2179.9</v>
+        <v>2802</v>
       </c>
       <c r="J10" s="1" t="n"/>
       <c r="K10" s="1" t="n"/>
@@ -699,13 +699,13 @@
         <v>0.4375</v>
       </c>
       <c r="G11" s="1" t="n">
-        <v>2184.9</v>
+        <v>2817.9</v>
       </c>
       <c r="H11" s="1" t="n">
-        <v>2170.1</v>
+        <v>2779.75</v>
       </c>
       <c r="I11" s="1" t="n">
-        <v>2173.15</v>
+        <v>2782.85</v>
       </c>
       <c r="J11" s="1" t="n"/>
       <c r="K11" s="1" t="n"/>
@@ -724,13 +724,13 @@
         <v>0.4583333333333333</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>2174.6</v>
+        <v>2798.15</v>
       </c>
       <c r="H12" s="1" t="n">
-        <v>2162.55</v>
+        <v>2767.1</v>
       </c>
       <c r="I12" s="1" t="n">
-        <v>2169.95</v>
+        <v>2795.4</v>
       </c>
       <c r="J12" s="1" t="n"/>
       <c r="K12" s="1" t="n"/>
@@ -749,13 +749,13 @@
         <v>0.4791666666666667</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>2171.2</v>
+        <v>2798.8</v>
       </c>
       <c r="H13" s="1" t="n">
-        <v>2165.3</v>
+        <v>2780</v>
       </c>
       <c r="I13" s="1" t="n">
-        <v>2168.45</v>
+        <v>2787.3</v>
       </c>
       <c r="J13" s="1" t="n"/>
       <c r="K13" s="1" t="n"/>
@@ -774,13 +774,13 @@
         <v>0.5</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>2169</v>
+        <v>2799</v>
       </c>
       <c r="H14" s="1" t="n">
-        <v>2166</v>
+        <v>2786.15</v>
       </c>
       <c r="I14" s="1" t="n">
-        <v>2167.25</v>
+        <v>2794.5</v>
       </c>
       <c r="J14" s="1" t="n"/>
       <c r="K14" s="1" t="n"/>
@@ -799,13 +799,13 @@
         <v>0.5208333333333334</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>2169.4</v>
+        <v>2805.95</v>
       </c>
       <c r="H15" s="1" t="n">
-        <v>2156.45</v>
+        <v>2789.05</v>
       </c>
       <c r="I15" s="1" t="n">
-        <v>2160.35</v>
+        <v>2795.4</v>
       </c>
       <c r="J15" s="1" t="n"/>
       <c r="K15" s="1" t="n"/>
@@ -824,13 +824,13 @@
         <v>0.5416666666666666</v>
       </c>
       <c r="G16" s="1" t="n">
-        <v>2163</v>
+        <v>2800.8</v>
       </c>
       <c r="H16" s="1" t="n">
-        <v>2157.1</v>
+        <v>2789</v>
       </c>
       <c r="I16" s="1" t="n">
-        <v>2159.8</v>
+        <v>2791.9</v>
       </c>
       <c r="J16" s="1" t="n"/>
       <c r="K16" s="1" t="n"/>
@@ -849,13 +849,13 @@
         <v>0.5625</v>
       </c>
       <c r="G17" s="1" t="n">
-        <v>2161.4</v>
+        <v>2798.9</v>
       </c>
       <c r="H17" s="1" t="n">
-        <v>2153.5</v>
+        <v>2785.1</v>
       </c>
       <c r="I17" s="1" t="n">
-        <v>2158.45</v>
+        <v>2798.4</v>
       </c>
       <c r="J17" s="1" t="n"/>
       <c r="K17" s="1" t="n"/>
@@ -874,13 +874,13 @@
         <v>0.5833333333333334</v>
       </c>
       <c r="G18" s="1" t="n">
-        <v>2161.45</v>
+        <v>2803.95</v>
       </c>
       <c r="H18" s="1" t="n">
-        <v>2158.05</v>
+        <v>2773</v>
       </c>
       <c r="I18" s="1" t="n">
-        <v>2160.1</v>
+        <v>2784.4</v>
       </c>
       <c r="J18" s="1" t="n"/>
       <c r="K18" s="1" t="n"/>
@@ -899,13 +899,13 @@
         <v>0.6041666666666666</v>
       </c>
       <c r="G19" s="1" t="n">
-        <v>2169</v>
+        <v>2791.95</v>
       </c>
       <c r="H19" s="1" t="n">
-        <v>2158</v>
+        <v>2777.1</v>
       </c>
       <c r="I19" s="1" t="n">
-        <v>2168.5</v>
+        <v>2778.95</v>
       </c>
       <c r="J19" s="1" t="n"/>
       <c r="K19" s="1" t="n"/>
@@ -924,13 +924,13 @@
         <v>0.625</v>
       </c>
       <c r="G20" s="1" t="n">
-        <v>2176.5</v>
+        <v>2787.45</v>
       </c>
       <c r="H20" s="1" t="n">
-        <v>2168.25</v>
+        <v>2774.2</v>
       </c>
       <c r="I20" s="1" t="n">
-        <v>2170.2</v>
+        <v>2776.85</v>
       </c>
       <c r="J20" s="1" t="n"/>
       <c r="K20" s="1" t="n"/>
@@ -949,13 +949,13 @@
         <v>0.6458333333333334</v>
       </c>
       <c r="G21" s="1" t="n">
-        <v>2176.45</v>
+        <v>2821.95</v>
       </c>
       <c r="H21" s="1" t="n">
-        <v>2168.6</v>
+        <v>2774</v>
       </c>
       <c r="I21" s="1" t="n">
-        <v>2175</v>
+        <v>2814</v>
       </c>
       <c r="J21" s="1" t="n"/>
       <c r="K21" s="1" t="n"/>

</xml_diff>